<commit_message>
without outofdomain and same prompt
</commit_message>
<xml_diff>
--- a/test_case/question_2categorylevel.xlsx
+++ b/test_case/question_2categorylevel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\agent_seniorProject\test_case\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\seniorProject\term2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A3C054-32A3-4EB1-B7D8-48623B300EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFDF7BD-F799-456D-AF7F-D0B9C963D5A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58260" yWindow="4725" windowWidth="13800" windowHeight="15585" xr2:uid="{E4F62F18-D066-4A55-BE5D-235A198FB64D}"/>
+    <workbookView xWindow="57495" yWindow="4725" windowWidth="14610" windowHeight="15585" xr2:uid="{E4F62F18-D066-4A55-BE5D-235A198FB64D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,6 +42,9 @@
     <t>category_level2</t>
   </si>
   <si>
+    <t xml:space="preserve">question </t>
+  </si>
+  <si>
     <t>หัตถการ</t>
   </si>
   <si>
@@ -196,9 +199,6 @@
   </si>
   <si>
     <t>หลังถอนฟันแล้ว ใช้น้ำยาบ้วนปากได้มั้ย</t>
-  </si>
-  <si>
-    <t>question</t>
   </si>
 </sst>
 </file>
@@ -588,7 +588,7 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -606,436 +606,436 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>